<commit_message>
Clean solution and documentation
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RequestPayments" sheetId="1" r:id="rId1"/>
-    <sheet name="GetPaymentDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="GetPaymentDetails" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Read payment details" sheetId="4" r:id="rId3"/>
-    <sheet name="Read payment details - 2" sheetId="5" r:id="rId4"/>
+    <sheet name="Read payment details - 2" sheetId="5" state="hidden" r:id="rId4"/>
     <sheet name="PC config" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>requests</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Parallel calls</t>
-  </si>
-  <si>
-    <t>When Kestrel max concurrent connections =1000</t>
   </si>
   <si>
     <t>Kestrel: Connection id "0HLNTNNE6J3M2" rejected because the maximum number of concurrent connections has been reached.</t>
@@ -407,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,110 +463,31 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1000</v>
-      </c>
-      <c r="B4">
-        <v>11.331</v>
-      </c>
-      <c r="C4" s="2">
-        <f t="shared" ref="C4:C13" si="0">B4/A4*1000*1000</f>
-        <v>11331</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" ref="D4:D13" si="1">A4/B4</f>
-        <v>88.253463948459981</v>
-      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D8" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D9" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D10" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D11" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D12" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D13" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="D12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -645,10 +563,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +777,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -883,38 +801,6 @@
       <c r="F10">
         <f t="shared" si="4"/>
         <v>0.32030365769496205</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>50</v>
-      </c>
-      <c r="B11">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1000</v>
-      </c>
-      <c r="B13">
-        <v>236</v>
-      </c>
-      <c r="E13" t="e">
-        <f>A13*B13/D13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13">
-        <f>D13/B13/A13*1000</f>
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -926,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>

</xml_diff>